<commit_message>
final commit of the day
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/BLJ-Project/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0806C12E-3A45-9D43-86EB-D151318D70F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F12178D-7829-F74C-BB06-01A3580796FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19980" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Nr.</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>A009</t>
+  </si>
+  <si>
+    <t>A010</t>
   </si>
 </sst>
 </file>
@@ -1771,7 +1774,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.999999999999996</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2278,8 +2281,8 @@
   </sheetPr>
   <dimension ref="A1:BJ45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="161" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="161" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3567,7 +3570,7 @@
       </c>
       <c r="D18" s="41">
         <f>SUM(D19:D33)</f>
-        <v>26.999999999999996</v>
+        <v>35</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="30"/>
@@ -3715,7 +3718,7 @@
       </c>
       <c r="D20" s="80">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20" s="49"/>
       <c r="F20" s="50"/>
@@ -3744,7 +3747,9 @@
       <c r="W20" s="54">
         <v>2</v>
       </c>
-      <c r="X20" s="54"/>
+      <c r="X20" s="54">
+        <v>2</v>
+      </c>
       <c r="Y20" s="55"/>
       <c r="Z20" s="56"/>
       <c r="AA20" s="57"/>
@@ -4096,7 +4101,7 @@
       </c>
       <c r="D25" s="80">
         <f t="shared" si="1"/>
-        <v>13.8</v>
+        <v>18.8</v>
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="50"/>
@@ -4123,7 +4128,9 @@
       <c r="W25" s="95">
         <v>6</v>
       </c>
-      <c r="X25" s="54"/>
+      <c r="X25" s="54">
+        <v>5</v>
+      </c>
       <c r="Y25" s="55"/>
       <c r="Z25" s="56"/>
       <c r="AA25" s="57"/>
@@ -4467,11 +4474,13 @@
       <c r="A30" s="12">
         <v>312</v>
       </c>
-      <c r="B30" s="45"/>
+      <c r="B30" s="45" t="s">
+        <v>61</v>
+      </c>
       <c r="C30" s="48"/>
       <c r="D30" s="80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="49"/>
       <c r="F30" s="50"/>
@@ -4492,7 +4501,9 @@
       <c r="U30" s="68"/>
       <c r="V30" s="69"/>
       <c r="W30" s="55"/>
-      <c r="X30" s="55"/>
+      <c r="X30" s="55">
+        <v>1</v>
+      </c>
       <c r="Y30" s="55"/>
       <c r="Z30" s="56"/>
       <c r="AA30" s="57"/>
@@ -5536,7 +5547,7 @@
       </c>
       <c r="D45" s="36">
         <f>D41+D38+D34+D18+D14+D9</f>
-        <v>31.999999999999996</v>
+        <v>40</v>
       </c>
       <c r="E45" s="36"/>
       <c r="F45" s="37"/>
@@ -5610,7 +5621,7 @@
       </c>
       <c r="X45" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y45" s="38">
         <f t="shared" si="4"/>
@@ -5868,7 +5879,7 @@
       </c>
       <c r="D5" s="77">
         <f>Zeitplanung!D18</f>
-        <v>26.999999999999996</v>
+        <v>35</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="78"/>

</xml_diff>